<commit_message>
este es el primer commit a la rama seba
</commit_message>
<xml_diff>
--- a/MODELO v4.xlsx
+++ b/MODELO v4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmass\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianguerreronunez/Desktop/Seba/Universidad/2020-1/Banca de Inversiones/Banca-de-Inversiones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC2D63F1-6BE6-4DE2-873E-9E6BD8F6BA99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02300EF-EDF0-B64F-A6A3-5219AE652BC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{20AA55B2-BE43-E14B-A8F4-38961449886A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19760" activeTab="8" xr2:uid="{20AA55B2-BE43-E14B-A8F4-38961449886A}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="290">
   <si>
     <t>Modelo de Valoración: Engie</t>
   </si>
@@ -905,6 +907,12 @@
   </si>
   <si>
     <t>Utilidad neta atribuible a prop?, paso 8 usa recurrente</t>
+  </si>
+  <si>
+    <t>ESTO ES ALGO QUE ESCRIBIO SEBA</t>
+  </si>
+  <si>
+    <t>ESTO ES ALGO QUE ESCRIBIO SEBA QUE SERÁ CONFLICTO</t>
   </si>
 </sst>
 </file>
@@ -912,15 +920,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="#,##0;\(#,##0\)"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0_);\(#,##0.0\);0.0_);@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000;\(#,##0.000\)"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="#,##0.0\x_);\(#,##0.0\x\);0.0_);@_)"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0;\(#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\);0.0_);@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000;\(#,##0.000\)"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0\x_);\(#,##0.0\x\);0.0_);@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1171,10 +1179,10 @@
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="172" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1217,14 +1225,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -1232,18 +1240,18 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="20" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="168" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
@@ -1253,41 +1261,41 @@
     <xf numFmtId="3" fontId="20" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="20" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="20" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="18" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="25" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="20" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="20" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="170" fontId="21" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
-    <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Moneda [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Times" xfId="5" xr:uid="{E4A581F4-CB3D-4AF6-BED0-4E104AF969C7}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1312,7 +1320,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="es-ES"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1349,7 +1357,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1389,7 +1397,7 @@
             <c:numRef>
               <c:f>Ventas!$S$23:$Y$23</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>44196</c:v>
@@ -1482,7 +1490,7 @@
             <c:numRef>
               <c:f>Ventas!$S$23:$Y$23</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>44196</c:v>
@@ -1575,7 +1583,7 @@
             <c:numRef>
               <c:f>Ventas!$S$23:$Y$23</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>44196</c:v>
@@ -1657,7 +1665,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1691,7 +1699,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="654091136"/>
@@ -1749,7 +1757,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-CL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="620775072"/>
@@ -1791,7 +1799,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-CL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1821,7 +1829,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="en-CL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2557,7 +2565,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2859,14 +2867,14 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="27.69921875" customWidth="1"/>
-    <col min="3" max="3" width="5.296875" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:15" ht="36.6">
+    <row r="3" spans="2:15" ht="37">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3031,16 +3039,16 @@
       <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="4.796875" customWidth="1"/>
-    <col min="3" max="3" width="44.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.296875" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="36.6">
+    <row r="1" spans="2:20" ht="37">
       <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
@@ -3081,7 +3089,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="23.4">
+    <row r="2" spans="2:20" ht="24">
       <c r="B2" s="11" t="s">
         <v>26</v>
       </c>
@@ -4201,20 +4209,20 @@
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="63.69921875" customWidth="1"/>
-    <col min="4" max="4" width="4.19921875" customWidth="1"/>
-    <col min="5" max="5" width="5.796875" customWidth="1"/>
-    <col min="6" max="6" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="36.6">
+    <row r="1" spans="2:16" ht="37">
       <c r="B1" s="7" t="str">
         <f>Cover!D5</f>
         <v xml:space="preserve">Engie Energía Chile </v>
@@ -4256,7 +4264,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="23.4">
+    <row r="2" spans="2:16" ht="24">
       <c r="B2" s="6" t="s">
         <v>19</v>
       </c>
@@ -5816,16 +5824,16 @@
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="4.796875" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="3" width="41" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5" customWidth="1"/>
-    <col min="5" max="5" width="6.19921875" customWidth="1"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="36.6">
+    <row r="1" spans="2:16" ht="37">
       <c r="B1" s="7" t="str">
         <f>Cover!D5</f>
         <v xml:space="preserve">Engie Energía Chile </v>
@@ -5867,7 +5875,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="23.4">
+    <row r="2" spans="2:16" ht="24">
       <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
@@ -6649,17 +6657,17 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="4.5" customWidth="1"/>
-    <col min="2" max="2" width="4.69921875" customWidth="1"/>
-    <col min="3" max="3" width="40.796875" customWidth="1"/>
-    <col min="4" max="4" width="4.296875" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="9" width="11.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="36.6">
+    <row r="1" spans="2:16" ht="37">
       <c r="B1" s="7" t="str">
         <f>Cover!D5</f>
         <v xml:space="preserve">Engie Energía Chile </v>
@@ -6701,7 +6709,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="23.4">
+    <row r="2" spans="2:16" ht="24">
       <c r="B2" s="6" t="s">
         <v>190</v>
       </c>
@@ -7419,21 +7427,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E81F22-0FF8-944B-ADDA-803A694294D1}">
   <dimension ref="A1:Q99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.69921875" customWidth="1"/>
-    <col min="2" max="2" width="2.69921875" customWidth="1"/>
-    <col min="3" max="3" width="42.796875" customWidth="1"/>
-    <col min="4" max="4" width="5.296875" customWidth="1"/>
-    <col min="5" max="5" width="4.69921875" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="2.6640625" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
+    <col min="4" max="4" width="5.33203125" customWidth="1"/>
+    <col min="5" max="5" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="36.6">
+    <row r="1" spans="1:17" ht="37">
       <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
@@ -7474,7 +7482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="23.4">
+    <row r="2" spans="1:17" ht="24">
       <c r="B2" s="11" t="s">
         <v>92</v>
       </c>
@@ -9137,16 +9145,16 @@
       <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.296875" customWidth="1"/>
-    <col min="2" max="2" width="3.796875" customWidth="1"/>
-    <col min="3" max="3" width="34.69921875" customWidth="1"/>
-    <col min="4" max="4" width="6.296875" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="36.6">
+    <row r="1" spans="2:16" ht="37">
       <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
@@ -9187,7 +9195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="23.4">
+    <row r="2" spans="2:16" ht="24">
       <c r="B2" s="11" t="s">
         <v>23</v>
       </c>
@@ -9257,17 +9265,17 @@
       <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.296875" customWidth="1"/>
-    <col min="2" max="2" width="3.796875" customWidth="1"/>
-    <col min="3" max="3" width="57.69921875" customWidth="1"/>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="3.83203125" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" customWidth="1"/>
     <col min="4" max="4" width="6.5" style="18" customWidth="1"/>
-    <col min="5" max="5" width="6.19921875" customWidth="1"/>
-    <col min="6" max="16" width="10.796875" style="27"/>
+    <col min="5" max="5" width="6.1640625" customWidth="1"/>
+    <col min="6" max="16" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="36.6">
+    <row r="1" spans="2:16" ht="37">
       <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
@@ -9308,7 +9316,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="23.4">
+    <row r="2" spans="2:16" ht="24">
       <c r="B2" s="11" t="s">
         <v>79</v>
       </c>
@@ -10340,17 +10348,17 @@
       <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.19921875" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="47.69921875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" style="18" customWidth="1"/>
-    <col min="5" max="5" width="6.69921875" style="18" customWidth="1"/>
+    <col min="3" max="3" width="47.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="18" customWidth="1"/>
     <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="36.6">
+    <row r="1" spans="2:16" ht="37">
       <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
@@ -10391,7 +10399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:16" ht="23.4">
+    <row r="2" spans="2:16" ht="24">
       <c r="B2" s="11" t="s">
         <v>24</v>
       </c>
@@ -16595,22 +16603,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043E3136-2CCC-4942-8CBF-640AE7E2E9F8}">
-  <dimension ref="B1:T45"/>
+  <dimension ref="B1:T50"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="4.5" customWidth="1"/>
-    <col min="3" max="3" width="73.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="5" max="5" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="36.6">
+    <row r="1" spans="2:20" ht="37">
       <c r="B1" s="9" t="s">
         <v>18</v>
       </c>
@@ -16651,7 +16659,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="23.4">
+    <row r="2" spans="2:20" ht="24">
       <c r="B2" s="11" t="s">
         <v>25</v>
       </c>
@@ -16737,7 +16745,7 @@
       <c r="S6" s="70"/>
       <c r="T6" s="70"/>
     </row>
-    <row r="7" spans="2:20" ht="31.2">
+    <row r="7" spans="2:20" ht="34">
       <c r="C7" s="72" t="s">
         <v>252</v>
       </c>
@@ -16923,7 +16931,7 @@
         <v>-35472</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="30.6" customHeight="1">
+    <row r="23" spans="2:9" ht="30.5" customHeight="1">
       <c r="C23" s="72" t="s">
         <v>266</v>
       </c>
@@ -16931,7 +16939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="31.8" customHeight="1">
+    <row r="24" spans="2:9" ht="31.75" customHeight="1">
       <c r="C24" s="72" t="s">
         <v>267</v>
       </c>
@@ -17044,7 +17052,7 @@
         <v>-131571</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="28.8" customHeight="1">
+    <row r="40" spans="2:10" ht="28.75" customHeight="1">
       <c r="C40" s="72" t="s">
         <v>279</v>
       </c>
@@ -17097,6 +17105,16 @@
       <c r="I45" s="73">
         <f>I42+I44</f>
         <v>239083</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" t="s">
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
volviendo a ser vacio
</commit_message>
<xml_diff>
--- a/MODELO v4.xlsx
+++ b/MODELO v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastianguerreronunez/Desktop/Seba/Universidad/2020-1/Banca de Inversiones/Banca-de-Inversiones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2966F55-2E6D-1D4A-829A-34405FB9F67D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B24F37A-6783-684D-952C-ACA4BDD604E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19740" activeTab="8" xr2:uid="{20AA55B2-BE43-E14B-A8F4-38961449886A}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="288">
   <si>
     <t>Modelo de Valoración: Engie</t>
   </si>
@@ -907,12 +907,6 @@
   </si>
   <si>
     <t>Utilidad neta atribuible a prop?, paso 8 usa recurrente</t>
-  </si>
-  <si>
-    <t>ESTO ES ALGO QUE ESCRIBIO ROBERTO</t>
-  </si>
-  <si>
-    <t>ESTO ES ALGO QUE ESCRIBIO ROBERTO QUE SERÁ CONFLICTO</t>
   </si>
 </sst>
 </file>
@@ -16603,11 +16597,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043E3136-2CCC-4942-8CBF-640AE7E2E9F8}">
-  <dimension ref="B1:T50"/>
+  <dimension ref="B1:T45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
+      <selection pane="bottomLeft" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17107,16 +17101,6 @@
         <v>239083</v>
       </c>
     </row>
-    <row r="49" spans="3:3">
-      <c r="C49" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" t="s">
-        <v>289</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>